<commit_message>
Endra costExport og costEnergy til activityCost med operational mode
</commit_message>
<xml_diff>
--- a/Input_data_With_dummyGrid_and_RT.xlsx
+++ b/Input_data_With_dummyGrid_and_RT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ojviken\OneDrive\Dokumenter\10. semester\Til master\Kjøre kode\14.05\Master_repo-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\V8\Master_repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188BF377-EDE3-4211-A352-064AFE2BC223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE35D3F4-1EA4-478C-984C-EF3E9D8BC619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="20" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="14" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -81,18 +81,36 @@
   <commentList>
     <comment ref="B6" authorId="0" shapeId="0" xr:uid="{FB04843D-B295-40BA-A00D-5E6B2A5753A5}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RT buy</t>
+        </r>
       </text>
     </comment>
     <comment ref="B7" authorId="1" shapeId="0" xr:uid="{5B616586-A621-4A9A-8B8B-B24C9A3AFD46}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RT sell</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -107,10 +125,19 @@
   <commentList>
     <comment ref="C37" authorId="0" shapeId="0" xr:uid="{C5776892-1F20-4F03-80A7-219BD90F0AD8}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RT sell</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -125,10 +152,19 @@
   <commentList>
     <comment ref="C5" authorId="0" shapeId="0" xr:uid="{FA6AF892-F62D-433D-A1F3-B906131A1ADB}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RT buy</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -143,10 +179,19 @@
   <commentList>
     <comment ref="C37" authorId="0" shapeId="0" xr:uid="{4AB2F2FD-D9AF-4EF6-975B-D27067AE3E61}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RT sell</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -161,10 +206,19 @@
   <commentList>
     <comment ref="C5" authorId="0" shapeId="0" xr:uid="{38A2CE00-8A9F-411D-8730-D3AF28BB4DFB}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RT buy</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -1547,7 +1601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -2149,7 +2203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -3277,7 +3331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -4087,7 +4141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -4783,7 +4837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A3:C55"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
@@ -6638,17 +6692,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEBC57C6511F094FB1659D4FD897CA2A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e300c8dce90f4bd359ffe07958d068a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5caa653f-10d0-46a2-81cc-01cb3798075e" xmlns:ns3="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="947f29ac9f688054ae1e7aaca14544db" ns2:_="" ns3:_="">
     <xsd:import namespace="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
@@ -6849,6 +6892,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6859,23 +6913,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6894,6 +6931,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
   <ds:schemaRefs>

</xml_diff>